<commit_message>
Overwrite contributions from DISA import. (#70)
* update contributions with disa import (daily)
</commit_message>
<xml_diff>
--- a/ok_tools/test_data/valid.xlsx
+++ b/ok_tools/test_data/valid.xlsx
@@ -194,10 +194,10 @@
   <dimension ref="B1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -409,7 +409,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Ignore contributions with specific prefix (#78)
like 'Trailer' or 'Programmvorschau'
</commit_message>
<xml_diff>
--- a/ok_tools/test_data/valid.xlsx
+++ b/ok_tools/test_data/valid.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t xml:space="preserve">Anfang</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t xml:space="preserve">Infoblock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programmvorschau2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trailer2022</t>
   </si>
 </sst>
 </file>
@@ -194,10 +200,10 @@
   <dimension ref="B1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -289,6 +295,64 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -409,7 +473,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>